<commit_message>
Add Data Driven Testing, Checkpoints, & Test Suites
</commit_message>
<xml_diff>
--- a/Data Files/SampleCity.xlsx
+++ b/Data Files/SampleCity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bsi90938\Documents\Katalon\Katalon-Automation-Portfolio\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147CD8B1-5028-425F-9DBF-8E01CE63017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715788D0-5D4B-4AD6-9ECD-3964C8F1D2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1224" yWindow="2388" windowWidth="17280" windowHeight="9420" xr2:uid="{5D189748-079C-415F-9016-049085867015}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Jakarta</t>
   </si>
   <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
     <t>Atlanta</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>expectedResult</t>
+  </si>
+  <si>
+    <t>Tokio</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,10 +456,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -474,20 +474,20 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1"/>
       <c r="J4" s="2"/>

</xml_diff>

<commit_message>
Add StudioAssist Use Case
</commit_message>
<xml_diff>
--- a/Data Files/SampleCity.xlsx
+++ b/Data Files/SampleCity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bsi90938\Documents\Katalon\Katalon-Automation-Portfolio\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bsi90938\Documents\Katalon dzikri.asa\Katalon-Automation-Portfolio\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715788D0-5D4B-4AD6-9ECD-3964C8F1D2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F1655D-DE47-4E9E-B01E-0B15BC1377FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1224" yWindow="2388" windowWidth="17280" windowHeight="9420" xr2:uid="{5D189748-079C-415F-9016-049085867015}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>expectedResult</t>
   </si>
   <si>
-    <t>Tokio</t>
+    <t>Tokyo</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>